<commit_message>
added new Passenger utils
</commit_message>
<xml_diff>
--- a/MakeMyTrip/TestData/InputData.xlsx
+++ b/MakeMyTrip/TestData/InputData.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\249079\source\repos\Selenium_MiniProject\MakeMyTrip\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB6A061-61EB-4E2C-8125-9089F1F33742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9700475-5643-4694-A9CB-1B01B55EDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchFlight" sheetId="1" r:id="rId1"/>
+    <sheet name="PassengerDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>frominput</t>
   </si>
@@ -59,13 +60,34 @@
   </si>
   <si>
     <t>Dec</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>mobilenumber</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>akash@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +100,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -98,15 +128,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +476,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CD5C6A-E264-4242-8029-A4D4DB21AA31}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>9876784563</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{C825BA4F-0A50-4CA1-9B8E-8CF4A3988B0A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>